<commit_message>
revised the correlation code for intersections
</commit_message>
<xml_diff>
--- a/models/sev_correlation.xlsx
+++ b/models/sev_correlation.xlsx
@@ -5,22 +5,23 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samyan\OneDrive - BYU\R\Crash_Severity_Correlations\R\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samyan\OneDrive - BYU\R\Crash_Severity_Correlations\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:40009_{78C558D7-A47C-443D-B0D2-01ECBFC27D3F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{5983EB62-CE4C-40C9-8420-FF7A1EF03748}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:40009_{78C558D7-A47C-443D-B0D2-01ECBFC27D3F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{F0313921-B7CB-48AA-9C22-FA3C4BD4DD16}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="sev_correlation" sheetId="1" r:id="rId1"/>
+    <sheet name="Segments" sheetId="1" r:id="rId1"/>
+    <sheet name="Intersections" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="30">
   <si>
     <t>crash_severity_id</t>
   </si>
@@ -89,6 +90,27 @@
   </si>
   <si>
     <t>4, 5</t>
+  </si>
+  <si>
+    <t>0.82          0.94    0.62               0.84              0.58       0.31         0.17         0.14       0.59</t>
+  </si>
+  <si>
+    <t>0.89          0.82    0.68               0.68              0.62       0.30         0.16         0.11       0.63</t>
+  </si>
+  <si>
+    <t>0.84          0.62    0.62               0.49              0.55       0.23         0.12         0.07       0.63</t>
+  </si>
+  <si>
+    <t>0.54          0.42    0.37               0.32              0.31       0.18         0.05         0.04       0.38</t>
+  </si>
+  <si>
+    <t>0.22          0.14    0.17               0.12              0.17       0.05         0.11         0.05       0.15</t>
+  </si>
+  <si>
+    <t>0.56          0.42    0.38               0.33              0.33       0.18         0.07         0.05       0.39</t>
+  </si>
+  <si>
+    <t>0.84          0.62    0.61               0.49              0.54       0.23         0.12         0.07       0.62</t>
   </si>
 </sst>
 </file>
@@ -652,7 +674,37 @@
     <cellStyle name="Total" xfId="18" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="15" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -702,7 +754,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>sev_correlation!$A$4</c:f>
+              <c:f>Segments!$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -723,7 +775,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>sev_correlation!$B$1:$J$1</c:f>
+              <c:f>Segments!$B$1:$J$1</c:f>
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
@@ -758,7 +810,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>sev_correlation!$B$4:$J$4</c:f>
+              <c:f>Segments!$B$4:$J$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -803,7 +855,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>sev_correlation!$A$5</c:f>
+              <c:f>Segments!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -824,7 +876,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>sev_correlation!$B$1:$J$1</c:f>
+              <c:f>Segments!$B$1:$J$1</c:f>
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
@@ -859,7 +911,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>sev_correlation!$B$5:$J$5</c:f>
+              <c:f>Segments!$B$5:$J$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -904,7 +956,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>sev_correlation!$A$6</c:f>
+              <c:f>Segments!$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -925,7 +977,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>sev_correlation!$B$1:$J$1</c:f>
+              <c:f>Segments!$B$1:$J$1</c:f>
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
@@ -960,7 +1012,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>sev_correlation!$B$6:$J$6</c:f>
+              <c:f>Segments!$B$6:$J$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1339,7 +1391,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>sev_correlation!$A$4</c:f>
+              <c:f>Segments!$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1360,7 +1412,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>sev_correlation!$B$1:$J$1</c:f>
+              <c:f>Segments!$B$1:$J$1</c:f>
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
@@ -1395,7 +1447,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>sev_correlation!$B$4:$J$4</c:f>
+              <c:f>Segments!$B$4:$J$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1440,7 +1492,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>sev_correlation!$A$5</c:f>
+              <c:f>Segments!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1461,7 +1513,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>sev_correlation!$B$1:$J$1</c:f>
+              <c:f>Segments!$B$1:$J$1</c:f>
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
@@ -1496,7 +1548,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>sev_correlation!$B$5:$J$5</c:f>
+              <c:f>Segments!$B$5:$J$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1541,7 +1593,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>sev_correlation!$A$6</c:f>
+              <c:f>Segments!$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1562,7 +1614,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>sev_correlation!$B$1:$J$1</c:f>
+              <c:f>Segments!$B$1:$J$1</c:f>
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
@@ -1597,7 +1649,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>sev_correlation!$B$6:$J$6</c:f>
+              <c:f>Segments!$B$6:$J$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -2032,415 +2084,11 @@
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>sev_correlation!$N$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>3</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>sev_correlation!$O$1:$W$1</c:f>
-              <c:strCache>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>Angle</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Front to Rear</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Head on</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Sideswipe Same Direction</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Sideswipe Opposite Direction</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Parked Vehicle</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Rear to Side</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Rear to Rear</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Single Vehicle</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>sev_correlation!$O$4:$W$4</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>0.78</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.74</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.68</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.68</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.59</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.22</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.45</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-48AF-4AD9-99B8-6B3C3D4ECFA8}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>sev_correlation!$N$5</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>4</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>sev_correlation!$O$1:$W$1</c:f>
-              <c:strCache>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>Angle</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Front to Rear</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Head on</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Sideswipe Same Direction</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Sideswipe Opposite Direction</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Parked Vehicle</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Rear to Side</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Rear to Rear</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Single Vehicle</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>sev_correlation!$O$5:$W$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>0.51</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.45</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.45</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.46</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.42</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.36</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.16</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.09</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.49</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-48AF-4AD9-99B8-6B3C3D4ECFA8}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>sev_correlation!$N$6</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>5</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>sev_correlation!$O$1:$W$1</c:f>
-              <c:strCache>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>Angle</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Front to Rear</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Head on</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Sideswipe Same Direction</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Sideswipe Opposite Direction</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Parked Vehicle</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Rear to Side</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Rear to Rear</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Single Vehicle</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>sev_correlation!$O$6:$W$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>0.24</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.27</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.22</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.26</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.21</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.09</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.06</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.4</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-48AF-4AD9-99B8-6B3C3D4ECFA8}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>sev_correlation!$N$7</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>4, 5</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent4"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>sev_correlation!$O$1:$W$1</c:f>
-              <c:strCache>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>Angle</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Front to Rear</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Head on</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Sideswipe Same Direction</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Sideswipe Opposite Direction</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Parked Vehicle</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Rear to Side</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Rear to Rear</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Single Vehicle</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>sev_correlation!$O$7:$W$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>0.51</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.45</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.46</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.46</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.43</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.37</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.16</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.09</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.54</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-48AF-4AD9-99B8-6B3C3D4ECFA8}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
           <c:idx val="4"/>
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>sev_correlation!$N$8</c:f>
+              <c:f>Segments!$N$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2461,7 +2109,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>sev_correlation!$O$1:$W$1</c:f>
+              <c:f>Segments!$O$1:$W$1</c:f>
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
@@ -2496,7 +2144,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>sev_correlation!$O$8:$W$8</c:f>
+              <c:f>Segments!$O$8:$W$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -2548,6 +2196,494 @@
         <c:overlap val="-27"/>
         <c:axId val="765913615"/>
         <c:axId val="1028066047"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Segments!$N$4</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>3</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Segments!$O$1:$W$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="9"/>
+                      <c:pt idx="0">
+                        <c:v>Angle</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Front to Rear</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Head on</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Sideswipe Same Direction</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>Sideswipe Opposite Direction</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>Parked Vehicle</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>Rear to Side</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>Rear to Rear</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>Single Vehicle</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Segments!$O$4:$W$4</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="9"/>
+                      <c:pt idx="0">
+                        <c:v>0.78</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.74</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.68</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.68</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0.59</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0.5</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>0.22</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>0.2</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>0.45</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000000-48AF-4AD9-99B8-6B3C3D4ECFA8}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Segments!$N$5</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>4</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent2"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Segments!$O$1:$W$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="9"/>
+                      <c:pt idx="0">
+                        <c:v>Angle</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Front to Rear</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Head on</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Sideswipe Same Direction</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>Sideswipe Opposite Direction</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>Parked Vehicle</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>Rear to Side</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>Rear to Rear</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>Single Vehicle</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Segments!$O$5:$W$5</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="9"/>
+                      <c:pt idx="0">
+                        <c:v>0.51</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.45</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.45</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.46</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0.42</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0.36</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>0.16</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>0.09</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>0.49</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000001-48AF-4AD9-99B8-6B3C3D4ECFA8}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="2"/>
+                <c:order val="2"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Segments!$N$6</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>5</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent3"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Segments!$O$1:$W$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="9"/>
+                      <c:pt idx="0">
+                        <c:v>Angle</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Front to Rear</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Head on</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Sideswipe Same Direction</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>Sideswipe Opposite Direction</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>Parked Vehicle</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>Rear to Side</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>Rear to Rear</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>Single Vehicle</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Segments!$O$6:$W$6</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="9"/>
+                      <c:pt idx="0">
+                        <c:v>0.24</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.2</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.27</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.22</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0.26</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0.21</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>0.09</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>0.06</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>0.4</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000002-48AF-4AD9-99B8-6B3C3D4ECFA8}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="3"/>
+                <c:order val="3"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Segments!$N$7</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>4, 5</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent4"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Segments!$O$1:$W$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="9"/>
+                      <c:pt idx="0">
+                        <c:v>Angle</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Front to Rear</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Head on</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Sideswipe Same Direction</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>Sideswipe Opposite Direction</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>Parked Vehicle</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>Rear to Side</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>Rear to Rear</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>Single Vehicle</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Segments!$O$7:$W$7</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="9"/>
+                      <c:pt idx="0">
+                        <c:v>0.51</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.45</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.46</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.46</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0.43</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0.37</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>0.16</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>0.09</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>0.54</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000003-48AF-4AD9-99B8-6B3C3D4ECFA8}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+          </c:ext>
+        </c:extLst>
       </c:barChart>
       <c:catAx>
         <c:axId val="765913615"/>
@@ -2774,51 +2910,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.7538569804115085"/>
-          <c:y val="0.15073632154941191"/>
-          <c:w val="0.1135394451715334"/>
-          <c:h val="0.21342955726618087"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="1"/>
-      <c:spPr>
-        <a:solidFill>
-          <a:schemeClr val="bg1"/>
-        </a:solidFill>
-        <a:ln w="12700">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -2860,7 +2951,471 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
-  <c:userShapes r:id="rId3"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Severity to Manner of Collision</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Correlation</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Intersections!$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3, 4, 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Intersections!$B$1:$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>Angle</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Front to Rear</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Head on</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Sideswipe Same Direction</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Sideswipe Opposite Direction</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Parked Vehicle</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Rear to Side</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Rear to Rear</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Single Vehicle</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Intersections!$B$8:$J$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.61</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.49</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.23</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.62</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-842A-4439-9588-D71698F53E95}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="765913615"/>
+        <c:axId val="1028066047"/>
+        <c:extLst/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="765913615"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Manner of Collision</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1028066047"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1028066047"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Pearson Correlation</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="765913615"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
@@ -2984,6 +3539,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
@@ -3995,6 +4590,509 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4613,49 +5711,46 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
-    <cdr:from>
-      <cdr:x>0.75477</cdr:x>
-      <cdr:y>0.09147</cdr:y>
-    </cdr:from>
-    <cdr:to>
-      <cdr:x>0.90463</cdr:x>
-      <cdr:y>0.1593</cdr:y>
-    </cdr:to>
-    <cdr:sp macro="" textlink="">
-      <cdr:nvSpPr>
-        <cdr:cNvPr id="2" name="TextBox 1">
-          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>33338</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2DCCB5AE-14A2-441D-8619-C9774C57F0D4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DC06F8D3-5D29-4580-A346-9062C3386885}"/>
             </a:ext>
           </a:extLst>
-        </cdr:cNvPr>
-        <cdr:cNvSpPr txBox="1"/>
-      </cdr:nvSpPr>
-      <cdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="5276850" y="423864"/>
-          <a:ext cx="1047750" cy="314325"/>
-        </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </cdr:spPr>
-      <cdr:txBody>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
-        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>Severity</a:t>
-          </a:r>
-        </a:p>
-      </cdr:txBody>
-    </cdr:sp>
-  </cdr:relSizeAnchor>
-</c:userShapes>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4958,8 +6053,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:W25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="AC27" sqref="AC27"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C10" workbookViewId="0">
+      <selection activeCell="Q55" sqref="Q55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5920,46 +7015,46 @@
         <v>21</v>
       </c>
       <c r="O24" s="3" t="str">
-        <f>IF(O8&gt;=0.95,"Perfect",IF(O8&gt;=0.5,"Strong",IF(O8&gt;=0.3,"Medium",IF(O8=0,"None","Small"))))</f>
+        <f t="shared" ref="O24:W24" si="8">IF(O8&gt;=0.95,"Perfect",IF(O8&gt;=0.5,"Strong",IF(O8&gt;=0.3,"Medium",IF(O8=0,"None","Small"))))</f>
         <v>Strong</v>
       </c>
       <c r="P24" s="3" t="str">
-        <f>IF(P8&gt;=0.95,"Perfect",IF(P8&gt;=0.5,"Strong",IF(P8&gt;=0.3,"Medium",IF(P8=0,"None","Small"))))</f>
+        <f t="shared" si="8"/>
         <v>Strong</v>
       </c>
       <c r="Q24" s="3" t="str">
-        <f>IF(Q8&gt;=0.95,"Perfect",IF(Q8&gt;=0.5,"Strong",IF(Q8&gt;=0.3,"Medium",IF(Q8=0,"None","Small"))))</f>
+        <f t="shared" si="8"/>
         <v>Strong</v>
       </c>
       <c r="R24" s="3" t="str">
-        <f>IF(R8&gt;=0.95,"Perfect",IF(R8&gt;=0.5,"Strong",IF(R8&gt;=0.3,"Medium",IF(R8=0,"None","Small"))))</f>
+        <f t="shared" si="8"/>
         <v>Strong</v>
       </c>
       <c r="S24" s="3" t="str">
-        <f>IF(S8&gt;=0.95,"Perfect",IF(S8&gt;=0.5,"Strong",IF(S8&gt;=0.3,"Medium",IF(S8=0,"None","Small"))))</f>
+        <f t="shared" si="8"/>
         <v>Strong</v>
       </c>
       <c r="T24" s="3" t="str">
-        <f>IF(T8&gt;=0.95,"Perfect",IF(T8&gt;=0.5,"Strong",IF(T8&gt;=0.3,"Medium",IF(T8=0,"None","Small"))))</f>
+        <f t="shared" si="8"/>
         <v>Strong</v>
       </c>
       <c r="U24" s="3" t="str">
-        <f>IF(U8&gt;=0.95,"Perfect",IF(U8&gt;=0.5,"Strong",IF(U8&gt;=0.3,"Medium",IF(U8=0,"None","Small"))))</f>
+        <f t="shared" si="8"/>
         <v>Small</v>
       </c>
       <c r="V24" s="3" t="str">
-        <f>IF(V8&gt;=0.95,"Perfect",IF(V8&gt;=0.5,"Strong",IF(V8&gt;=0.3,"Medium",IF(V8=0,"None","Small"))))</f>
+        <f t="shared" si="8"/>
         <v>Small</v>
       </c>
       <c r="W24" s="3" t="str">
-        <f>IF(W8&gt;=0.95,"Perfect",IF(W8&gt;=0.5,"Strong",IF(W8&gt;=0.3,"Medium",IF(W8=0,"None","Small"))))</f>
+        <f t="shared" si="8"/>
         <v>Medium</v>
       </c>
     </row>
     <row r="25" spans="14:23" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="O18:W24">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"Strong"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5980,4 +7075,688 @@
   </ignoredErrors>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C22405F6-FFCB-4199-A651-5A7B4CFA8434}">
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1:J33"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A17" activeCellId="1" sqref="A1:J8 A17:J24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="10" width="10.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.94</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.62</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0.84</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0.31</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0.17</v>
+      </c>
+      <c r="I2" s="2">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="J2" s="2">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.89</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.68</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.68</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0.62</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0.16</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0.11</v>
+      </c>
+      <c r="J3" s="2">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.84</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.62</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.62</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.49</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0.23</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0.12</v>
+      </c>
+      <c r="I4" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="J4" s="2">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.54</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.42</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.37</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.32</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0.31</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0.18</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0.04</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.22</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.17</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.12</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.17</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0.11</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.42</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.38</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.33</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.33</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0.18</v>
+      </c>
+      <c r="H7" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="J7" s="2">
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.84</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.62</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.61</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.49</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0.54</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0.23</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="I8" s="3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="J8" s="3">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+    </row>
+    <row r="17" spans="1:10" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>1</v>
+      </c>
+      <c r="B18" s="2" t="str">
+        <f>IF(B2&gt;=0.95,"Perfect",IF(B2&gt;=0.5,"Strong",IF(B2&gt;=0.3,"Medium",IF(B2=0,"None","Small"))))</f>
+        <v>Strong</v>
+      </c>
+      <c r="C18" s="2" t="str">
+        <f t="shared" ref="C18:J18" si="0">IF(C2&gt;=0.95,"Perfect",IF(C2&gt;=0.5,"Strong",IF(C2&gt;=0.3,"Medium",IF(C2=0,"None","Small"))))</f>
+        <v>Strong</v>
+      </c>
+      <c r="D18" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Strong</v>
+      </c>
+      <c r="E18" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Strong</v>
+      </c>
+      <c r="F18" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Strong</v>
+      </c>
+      <c r="G18" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Medium</v>
+      </c>
+      <c r="H18" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Small</v>
+      </c>
+      <c r="I18" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Small</v>
+      </c>
+      <c r="J18" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Strong</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>2</v>
+      </c>
+      <c r="B19" s="2" t="str">
+        <f t="shared" ref="B19:J24" si="1">IF(B3&gt;=0.95,"Perfect",IF(B3&gt;=0.5,"Strong",IF(B3&gt;=0.3,"Medium",IF(B3=0,"None","Small"))))</f>
+        <v>Strong</v>
+      </c>
+      <c r="C19" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Strong</v>
+      </c>
+      <c r="D19" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Strong</v>
+      </c>
+      <c r="E19" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Strong</v>
+      </c>
+      <c r="F19" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Strong</v>
+      </c>
+      <c r="G19" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Medium</v>
+      </c>
+      <c r="H19" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Small</v>
+      </c>
+      <c r="I19" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Small</v>
+      </c>
+      <c r="J19" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Strong</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>3</v>
+      </c>
+      <c r="B20" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Strong</v>
+      </c>
+      <c r="C20" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Strong</v>
+      </c>
+      <c r="D20" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Strong</v>
+      </c>
+      <c r="E20" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Medium</v>
+      </c>
+      <c r="F20" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Strong</v>
+      </c>
+      <c r="G20" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Small</v>
+      </c>
+      <c r="H20" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Small</v>
+      </c>
+      <c r="I20" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Small</v>
+      </c>
+      <c r="J20" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Strong</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>4</v>
+      </c>
+      <c r="B21" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Strong</v>
+      </c>
+      <c r="C21" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Medium</v>
+      </c>
+      <c r="D21" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Medium</v>
+      </c>
+      <c r="E21" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Medium</v>
+      </c>
+      <c r="F21" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Medium</v>
+      </c>
+      <c r="G21" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Small</v>
+      </c>
+      <c r="H21" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Small</v>
+      </c>
+      <c r="I21" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Small</v>
+      </c>
+      <c r="J21" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Medium</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>5</v>
+      </c>
+      <c r="B22" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Small</v>
+      </c>
+      <c r="C22" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Small</v>
+      </c>
+      <c r="D22" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Small</v>
+      </c>
+      <c r="E22" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Small</v>
+      </c>
+      <c r="F22" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Small</v>
+      </c>
+      <c r="G22" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Small</v>
+      </c>
+      <c r="H22" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Small</v>
+      </c>
+      <c r="I22" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Small</v>
+      </c>
+      <c r="J22" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Small</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Strong</v>
+      </c>
+      <c r="C23" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Medium</v>
+      </c>
+      <c r="D23" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Medium</v>
+      </c>
+      <c r="E23" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Medium</v>
+      </c>
+      <c r="F23" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Medium</v>
+      </c>
+      <c r="G23" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Small</v>
+      </c>
+      <c r="H23" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Small</v>
+      </c>
+      <c r="I23" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Small</v>
+      </c>
+      <c r="J23" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Medium</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Strong</v>
+      </c>
+      <c r="C24" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Strong</v>
+      </c>
+      <c r="D24" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Strong</v>
+      </c>
+      <c r="E24" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Medium</v>
+      </c>
+      <c r="F24" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Strong</v>
+      </c>
+      <c r="G24" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Small</v>
+      </c>
+      <c r="H24" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Small</v>
+      </c>
+      <c r="I24" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Small</v>
+      </c>
+      <c r="J24" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Strong</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B18:J24">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"Strong"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:J8">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>